<commit_message>
Turklerin temmuz avansini hazirana gecirdim.
</commit_message>
<xml_diff>
--- a/Ofis Dosyalari/HAKEDISLER/2025/HAZIRAN 2025/2025 HAZIRAN AYI - TURKLER.xlsx
+++ b/Ofis Dosyalari/HAKEDISLER/2025/HAZIRAN 2025/2025 HAZIRAN AYI - TURKLER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samil\OneDrive\Masaüstü\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\OfisDosyalariYedegi\Ofis Dosyalari\HAKEDISLER\2025\HAZIRAN 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDB0E0F-4606-46A5-9A01-588934038A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8868683-10A0-43DF-BE18-8AF3FF45BBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="30" windowWidth="28755" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -678,6 +676,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -687,14 +686,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="ParaBirimi 2" xfId="3" xr:uid="{FB247420-4A8B-46B8-AD14-047A5DA77D80}"/>
     <cellStyle name="ParaBirimi 3" xfId="4" xr:uid="{BF168A53-9392-4368-8CBE-852921DB8D90}"/>
     <cellStyle name="ParaBirimi 4" xfId="2" xr:uid="{888C2C55-0B34-4D51-85C7-3866F707377C}"/>
     <cellStyle name="ParaBirimi 5" xfId="1" xr:uid="{EE63A87A-5B93-493C-B961-DE1FE32CA3E6}"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -975,39 +973,39 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A1" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="37"/>
-    </row>
-    <row r="2" spans="1:11" ht="43.8" thickBot="1">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="38"/>
+    </row>
+    <row r="2" spans="1:11" ht="45.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1058,13 +1056,15 @@
         <v>2500</v>
       </c>
       <c r="G3" s="23">
-        <f>F3*K3</f>
+        <f t="shared" ref="G3:G15" si="0">F3*K3</f>
         <v>202500</v>
       </c>
-      <c r="H3" s="23"/>
+      <c r="H3" s="23">
+        <v>10000</v>
+      </c>
       <c r="I3" s="23">
         <f>G3-H3</f>
-        <v>202500</v>
+        <v>192500</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="32">
@@ -1087,15 +1087,15 @@
         <v>2500</v>
       </c>
       <c r="G4" s="22">
-        <f>F4*K4</f>
+        <f t="shared" si="0"/>
         <v>202500</v>
       </c>
       <c r="H4" s="22">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="I4" s="22">
-        <f t="shared" ref="I4:I15" si="0">G4-H4</f>
-        <v>197500</v>
+        <f t="shared" ref="I4:I15" si="1">G4-H4</f>
+        <v>187500</v>
       </c>
       <c r="J4" s="28"/>
       <c r="K4" s="33">
@@ -1123,13 +1123,15 @@
         <v>2457</v>
       </c>
       <c r="G5" s="22">
-        <f>F5*K5</f>
-        <v>199017</v>
-      </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22">
         <f t="shared" si="0"/>
         <v>199017</v>
+      </c>
+      <c r="H5" s="22">
+        <v>5000</v>
+      </c>
+      <c r="I5" s="22">
+        <f t="shared" si="1"/>
+        <v>194017</v>
       </c>
       <c r="J5" s="28"/>
       <c r="K5" s="33">
@@ -1153,17 +1155,19 @@
         <v>7</v>
       </c>
       <c r="F6" s="12">
-        <f t="shared" ref="F6:F9" si="1">D6*E6</f>
+        <f t="shared" ref="F6:F9" si="2">D6*E6</f>
         <v>2548</v>
       </c>
       <c r="G6" s="22">
-        <f>F6*K6</f>
-        <v>206388</v>
-      </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22">
         <f t="shared" si="0"/>
         <v>206388</v>
+      </c>
+      <c r="H6" s="22">
+        <v>5000</v>
+      </c>
+      <c r="I6" s="22">
+        <f t="shared" si="1"/>
+        <v>201388</v>
       </c>
       <c r="J6" s="28"/>
       <c r="K6" s="33">
@@ -1187,16 +1191,16 @@
         <v>6</v>
       </c>
       <c r="F7" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2262</v>
       </c>
       <c r="G7" s="22">
-        <f>F7*K7</f>
+        <f t="shared" si="0"/>
         <v>183222</v>
       </c>
       <c r="H7" s="22"/>
       <c r="I7" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>183222</v>
       </c>
       <c r="J7" s="28"/>
@@ -1221,17 +1225,19 @@
         <v>7</v>
       </c>
       <c r="F8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2541</v>
       </c>
       <c r="G8" s="22">
-        <f>F8*K8</f>
-        <v>205821</v>
-      </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22">
         <f t="shared" si="0"/>
         <v>205821</v>
+      </c>
+      <c r="H8" s="22">
+        <v>5000</v>
+      </c>
+      <c r="I8" s="22">
+        <f t="shared" si="1"/>
+        <v>200821</v>
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="33">
@@ -1255,17 +1261,19 @@
         <v>7</v>
       </c>
       <c r="F9" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2317</v>
       </c>
       <c r="G9" s="22">
-        <f>F9*K9</f>
-        <v>187677</v>
-      </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22">
         <f t="shared" si="0"/>
         <v>187677</v>
+      </c>
+      <c r="H9" s="22">
+        <v>5000</v>
+      </c>
+      <c r="I9" s="22">
+        <f t="shared" si="1"/>
+        <v>182677</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="33">
@@ -1288,15 +1296,15 @@
         <v>2000</v>
       </c>
       <c r="G10" s="22">
-        <f>F10*K10</f>
+        <f t="shared" si="0"/>
         <v>162000</v>
       </c>
       <c r="H10" s="22">
-        <v>3000</v>
+        <v>13000</v>
       </c>
       <c r="I10" s="22">
-        <f t="shared" si="0"/>
-        <v>159000</v>
+        <f t="shared" si="1"/>
+        <v>149000</v>
       </c>
       <c r="J10" s="28"/>
       <c r="K10" s="33">
@@ -1324,12 +1332,12 @@
         <v>2380</v>
       </c>
       <c r="G11" s="22">
-        <f>F11*K11</f>
+        <f t="shared" si="0"/>
         <v>192780</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>192780</v>
       </c>
       <c r="J11" s="28"/>
@@ -1354,16 +1362,16 @@
         <v>7</v>
       </c>
       <c r="F12" s="12">
-        <f t="shared" ref="F12:F13" si="2">D12*E12</f>
+        <f t="shared" ref="F12:F13" si="3">D12*E12</f>
         <v>1708</v>
       </c>
       <c r="G12" s="22">
-        <f>F12*K12</f>
+        <f t="shared" si="0"/>
         <v>138348</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>138348</v>
       </c>
       <c r="J12" s="28"/>
@@ -1388,16 +1396,16 @@
         <v>6</v>
       </c>
       <c r="F13" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1848</v>
       </c>
       <c r="G13" s="22">
-        <f>F13*K13</f>
+        <f t="shared" si="0"/>
         <v>149688</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>149688</v>
       </c>
       <c r="J13" s="28"/>
@@ -1421,12 +1429,12 @@
         <v>2000</v>
       </c>
       <c r="G14" s="22">
-        <f>F14*K14</f>
+        <f t="shared" si="0"/>
         <v>162000</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162000</v>
       </c>
       <c r="J14" s="29"/>
@@ -1434,7 +1442,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1">
       <c r="A15" s="17">
         <v>13</v>
       </c>
@@ -1450,12 +1458,12 @@
         <v>2000</v>
       </c>
       <c r="G15" s="25">
-        <f>F15*K15</f>
+        <f t="shared" si="0"/>
         <v>162000</v>
       </c>
       <c r="H15" s="25"/>
       <c r="I15" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162000</v>
       </c>
       <c r="J15" s="30"/>
@@ -1463,17 +1471,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1"/>
-    <row r="17" spans="6:9" ht="15" thickBot="1">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="17" spans="6:9" ht="15.75" thickBot="1">
       <c r="F17" s="31">
         <f>SUM(F3:F16)</f>
         <v>29061</v>
       </c>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
       <c r="I17" s="26">
         <f>SUM(I3:I16)</f>
-        <v>2345941</v>
+        <v>2295941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>